<commit_message>
Add gallery view and example presets to app
Introduces a gallery view for browsing and selecting example remote label presets. Refactors App.tsx to support view switching between editor and gallery, updates CSS for gallery layout, and extends the RemoteExample type and remotes data to support button strikethrough overlays. Also updates RemoteSvg to support configurable backgrounds for gallery thumbnails.
</commit_message>
<xml_diff>
--- a/tools/remotes-calculation.xlsx
+++ b/tools/remotes-calculation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10102"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10118"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tgermer/git/ha-remote-labeler/tools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BF8D301-8275-B14D-B5B8-E7B380C69612}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D83F054B-4347-DA42-A22B-CA423175FE18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11580" yWindow="5460" windowWidth="28040" windowHeight="17240" xr2:uid="{259368C1-F00B-6B49-A5F9-87DEA9BCB168}"/>
+    <workbookView xWindow="2200" yWindow="2400" windowWidth="28040" windowHeight="17240" xr2:uid="{259368C1-F00B-6B49-A5F9-87DEA9BCB168}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -421,15 +421,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74DBA95A-F005-454F-9510-166AE4103BB3}">
-  <dimension ref="B3:F13"/>
+  <dimension ref="B3:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -437,23 +437,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B4" s="1">
         <v>1.8</v>
       </c>
       <c r="E4" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B5">
         <v>27</v>
       </c>
       <c r="E5">
         <v>28.5</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="H5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B6">
         <v>1.8</v>
       </c>
@@ -468,16 +474,26 @@
         <f>E4+E5+E6</f>
         <v>29.25</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1">
+        <f>H4+H5+H6</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B7" s="1">
         <v>16</v>
       </c>
       <c r="E7" s="1">
         <v>16.25</v>
       </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="H7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B8">
         <v>1.8</v>
       </c>
@@ -492,16 +508,26 @@
         <f>F6+E7+E8</f>
         <v>45.5</v>
       </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1">
+        <f>I6+H7+H8</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B9" s="1">
         <v>16</v>
       </c>
       <c r="E9" s="1">
         <v>16.25</v>
       </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="H9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B10">
         <v>1.8</v>
       </c>
@@ -516,16 +542,27 @@
         <f>F8+E9+E10</f>
         <v>62.5</v>
       </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10" s="1">
+        <f>I8+H9+H10</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B11" s="1">
         <v>27</v>
       </c>
       <c r="E11" s="1">
         <v>28.5</v>
       </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="H11" s="1">
+        <f>SUM(H4:H10)</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B12">
         <v>1.8</v>
       </c>
@@ -533,7 +570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B13">
         <f>SUM(B4:B12)</f>
         <v>95</v>

</xml_diff>